<commit_message>
updates from Sam: code setup; mine_heat fix; plots
</commit_message>
<xml_diff>
--- a/data/LMM_2a-D.xlsx
+++ b/data/LMM_2a-D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mikey\Documents\code_master\code_master\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonty\Desktop\ES into Industry\Industry project\mine_geothermal_code_ensemble2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7B2A73-AA0F-494A-867C-2339CB600D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF763120-9F73-484E-A079-44A1738CA972}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A3649537-06D5-4A14-9E8A-52B5EE3B5F09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{A3649537-06D5-4A14-9E8A-52B5EE3B5F09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9105F982-BDA5-48C7-9228-5E85AA790FDC}">
   <dimension ref="A1:EN205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113:XFD113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>